<commit_message>
Added image scale and colormap parameters to the datasets.
</commit_message>
<xml_diff>
--- a/10050_0270.xlsx
+++ b/10050_0270.xlsx
@@ -544,7 +544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,6 +598,86 @@
           <t>3.5-micron Filter</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>I4 Low Pixel Limit</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>I4 High Pixel Limit</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>I2 Low Pixel Limit</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>I2 High Pixel Limit</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>I1 Low Pixel Limit</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>I1 High Pixel Limit</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>I3 Low Pixel Limit</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>I3 High Pixel Limit</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>I4 Contrast</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>I4 Bias</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>I2 Contrast</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>I2 Bias</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>I1 Contrast</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>I1 Bias</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>I3 Contrast</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>I3 Bias</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -640,6 +720,54 @@
         <is>
           <t>cuts/101.0166378,3.0476406_10050_0270_Azul-3.5micras.jpeg</t>
         </is>
+      </c>
+      <c r="J2" t="n">
+        <v>5.63551</v>
+      </c>
+      <c r="K2" t="n">
+        <v>11.0478</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.170264</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.11561</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-0.320132</v>
+      </c>
+      <c r="O2" t="n">
+        <v>3.357</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-0.320132</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>14.1618</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.993151</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.4520547945205479</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1.09589</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="X2" t="n">
+        <v>1.23288</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.414384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>